<commit_message>
Multiple Modifications to the Files
</commit_message>
<xml_diff>
--- a/Python_Methods.xlsx
+++ b/Python_Methods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\myNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049E7D1A-EC32-40E5-B0FD-D9D4034F98B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63645FFE-282C-4E07-B409-AE5F319C9177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="String Methods(47)" sheetId="1" r:id="rId1"/>
@@ -2682,22 +2682,23 @@
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="2.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>360</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>123</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="27"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -2755,7 +2756,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="27"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -2773,7 +2774,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="27"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -2791,7 +2792,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="27"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -2809,7 +2810,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="27"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -2827,7 +2828,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="27" t="s">
         <v>122</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A9" s="27"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -2890,7 +2891,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="27"/>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -2935,7 +2936,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="27"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -2978,7 +2979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="27"/>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -2996,7 +2997,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="27"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -3012,7 +3013,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="27"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
@@ -3030,7 +3031,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>121</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="27"/>
       <c r="B16" s="2" t="s">
         <v>19</v>
@@ -3066,7 +3067,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="27"/>
       <c r="B17" s="2" t="s">
         <v>20</v>
@@ -3082,7 +3083,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="27"/>
       <c r="B18" s="2" t="s">
         <v>21</v>
@@ -3101,7 +3102,7 @@
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="27"/>
       <c r="B19" s="2" t="s">
         <v>22</v>
@@ -3120,7 +3121,7 @@
       </c>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="27"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -3138,7 +3139,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="27"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
@@ -3156,7 +3157,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
         <v>126</v>
@@ -3174,7 +3175,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="27"/>
       <c r="B23" s="2" t="s">
         <v>128</v>
@@ -3192,7 +3193,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="27" t="s">
         <v>132</v>
       </c>
@@ -3212,7 +3213,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="27"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
@@ -3230,7 +3231,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="27"/>
       <c r="B26" s="2" t="s">
         <v>27</v>
@@ -3248,7 +3249,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" s="27"/>
       <c r="B27" s="2" t="s">
         <v>28</v>
@@ -3266,7 +3267,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="27"/>
       <c r="B28" s="2" t="s">
         <v>29</v>
@@ -3284,7 +3285,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="27"/>
       <c r="B29" s="2" t="s">
         <v>133</v>
@@ -3302,7 +3303,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="27"/>
       <c r="B30" s="2" t="s">
         <v>30</v>
@@ -3320,7 +3321,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="27"/>
       <c r="B31" s="2" t="s">
         <v>31</v>
@@ -3338,7 +3339,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="27"/>
       <c r="B32" s="2" t="s">
         <v>32</v>
@@ -3356,7 +3357,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="27"/>
       <c r="B33" s="2" t="s">
         <v>33</v>
@@ -3374,7 +3375,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="27"/>
       <c r="B34" s="2" t="s">
         <v>34</v>
@@ -3392,7 +3393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="27"/>
       <c r="B35" s="2" t="s">
         <v>35</v>
@@ -3408,7 +3409,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="29" t="s">
         <v>120</v>
       </c>
@@ -3428,7 +3429,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="29"/>
       <c r="B37" s="2" t="s">
         <v>37</v>
@@ -3446,7 +3447,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="29"/>
       <c r="B38" s="2" t="s">
         <v>135</v>
@@ -3464,7 +3465,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="29"/>
       <c r="B39" s="2" t="s">
         <v>136</v>
@@ -3482,7 +3483,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="29"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
@@ -3500,7 +3501,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="29"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
@@ -3518,7 +3519,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="29"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
@@ -3536,7 +3537,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="27" t="s">
         <v>124</v>
       </c>
@@ -3556,7 +3557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="27"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
@@ -3572,7 +3573,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="27"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
@@ -3590,7 +3591,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="27"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
@@ -3606,7 +3607,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="27"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
@@ -3624,7 +3625,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="27"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
@@ -3642,7 +3643,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="27"/>
       <c r="B49" s="2" t="s">
         <v>47</v>
@@ -3660,7 +3661,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="27"/>
       <c r="B50" s="2" t="s">
         <v>48</v>
@@ -3678,7 +3679,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="27" t="s">
         <v>125</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="27"/>
       <c r="B52" s="2" t="s">
         <v>50</v>
@@ -3716,7 +3717,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="27"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
@@ -3734,7 +3735,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="27" t="s">
         <v>139</v>
       </c>
@@ -3754,7 +3755,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="27"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
@@ -3772,7 +3773,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A56" s="28"/>
       <c r="B56" s="4" t="s">
         <v>140</v>
@@ -3814,21 +3815,22 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3848,7 +3850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="30" t="s">
         <v>275</v>
       </c>
@@ -3868,7 +3870,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>279</v>
@@ -3886,7 +3888,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>283</v>
@@ -3904,7 +3906,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>287</v>
@@ -3922,7 +3924,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>290</v>
@@ -3940,7 +3942,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>152</v>
@@ -3958,7 +3960,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="30" t="s">
         <v>295</v>
       </c>
@@ -3978,7 +3980,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>298</v>
@@ -3996,7 +3998,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="30" t="s">
         <v>302</v>
       </c>
@@ -4016,7 +4018,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="30" t="s">
         <v>302</v>
       </c>
@@ -4036,7 +4038,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>310</v>
       </c>
@@ -4056,57 +4058,57 @@
         <v>312</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
         <v>371</v>
       </c>
@@ -4129,18 +4131,19 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -4154,7 +4157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>157</v>
       </c>
@@ -4168,7 +4171,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>160</v>
       </c>
@@ -4182,7 +4185,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="31" t="s">
         <v>164</v>
       </c>
@@ -4190,19 +4193,19 @@
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -4223,21 +4226,22 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4257,7 +4261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="30" t="s">
         <v>166</v>
       </c>
@@ -4277,7 +4281,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>168</v>
@@ -4295,7 +4299,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>169</v>
@@ -4313,7 +4317,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>170</v>
@@ -4331,7 +4335,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>151</v>
@@ -4349,7 +4353,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>152</v>
@@ -4367,7 +4371,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="30" t="s">
         <v>186</v>
       </c>
@@ -4387,7 +4391,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>190</v>
@@ -4405,7 +4409,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
         <v>193</v>
@@ -4423,7 +4427,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>197</v>
@@ -4441,7 +4445,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="30"/>
       <c r="B13" s="2" t="s">
         <v>201</v>
@@ -4459,7 +4463,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="30"/>
       <c r="B14" s="2" t="s">
         <v>204</v>
@@ -4477,7 +4481,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="30"/>
       <c r="B15" s="2" t="s">
         <v>207</v>
@@ -4495,7 +4499,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="30" t="s">
         <v>210</v>
       </c>
@@ -4515,7 +4519,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>218</v>
@@ -4533,7 +4537,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="30"/>
       <c r="B19" s="2" t="s">
         <v>221</v>
@@ -4551,7 +4555,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>211</v>
       </c>
@@ -4589,20 +4593,21 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4622,7 +4627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="30" t="s">
         <v>271</v>
       </c>
@@ -4642,7 +4647,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>229</v>
@@ -4660,7 +4665,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>233</v>
@@ -4678,7 +4683,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>237</v>
@@ -4696,7 +4701,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>241</v>
@@ -4714,7 +4719,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="30" t="s">
         <v>272</v>
       </c>
@@ -4734,7 +4739,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>250</v>
@@ -4752,7 +4757,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="30" t="s">
         <v>273</v>
       </c>
@@ -4772,7 +4777,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>257</v>
@@ -4790,7 +4795,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="30"/>
       <c r="B13" s="2" t="s">
         <v>261</v>
@@ -4808,7 +4813,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="30" t="s">
         <v>274</v>
       </c>
@@ -4828,7 +4833,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="30"/>
       <c r="B16" s="2" t="s">
         <v>267</v>
@@ -4864,22 +4869,23 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="33.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="112" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4899,7 +4905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="30" t="s">
         <v>569</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="30"/>
       <c r="B3" s="2" t="s">
         <v>378</v>
@@ -4937,7 +4943,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>383</v>
@@ -4955,7 +4961,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>387</v>
@@ -4973,7 +4979,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>390</v>
@@ -4991,7 +4997,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>394</v>
@@ -5009,7 +5015,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="30"/>
       <c r="B8" s="2" t="s">
         <v>398</v>
@@ -5027,7 +5033,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>401</v>
@@ -5045,7 +5051,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>405</v>
@@ -5063,7 +5069,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="30" t="s">
         <v>610</v>
       </c>
@@ -5083,7 +5089,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="30"/>
       <c r="B13" s="2" t="s">
         <v>419</v>
@@ -5101,7 +5107,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="30"/>
       <c r="B14" s="2" t="s">
         <v>414</v>
@@ -5119,7 +5125,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="30"/>
       <c r="B15" s="2" t="s">
         <v>429</v>
@@ -5137,7 +5143,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="30"/>
       <c r="B16" s="2" t="s">
         <v>434</v>
@@ -5155,7 +5161,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="30"/>
       <c r="B17" s="2" t="s">
         <v>612</v>
@@ -5173,7 +5179,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>461</v>
@@ -5191,7 +5197,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="30"/>
       <c r="B19" s="2" t="s">
         <v>466</v>
@@ -5209,7 +5215,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="30"/>
       <c r="B20" s="2" t="s">
         <v>424</v>
@@ -5227,7 +5233,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="32" t="s">
         <v>570</v>
       </c>
@@ -5247,7 +5253,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="33"/>
       <c r="B23" s="2" t="s">
         <v>443</v>
@@ -5265,7 +5271,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="33"/>
       <c r="B24" s="2" t="s">
         <v>446</v>
@@ -5283,7 +5289,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="33"/>
       <c r="B25" s="2" t="s">
         <v>450</v>
@@ -5301,7 +5307,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="34"/>
       <c r="B26" s="2" t="s">
         <v>454</v>
@@ -5319,10 +5325,10 @@
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="22"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="30" t="s">
         <v>628</v>
       </c>
@@ -5342,7 +5348,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="30"/>
       <c r="B29" s="2" t="s">
         <v>459</v>
@@ -5360,7 +5366,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="30"/>
       <c r="B30" s="2" t="s">
         <v>602</v>
@@ -5378,10 +5384,10 @@
         <v>605</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="24"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="30" t="s">
         <v>588</v>
       </c>
@@ -5401,7 +5407,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="30"/>
       <c r="B33" s="2" t="s">
         <v>573</v>
@@ -5419,7 +5425,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="30"/>
       <c r="B34" s="2" t="s">
         <v>575</v>
@@ -5438,7 +5444,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="30"/>
       <c r="B35" s="2" t="s">
         <v>577</v>
@@ -5456,10 +5462,10 @@
         <v>583</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="32" t="s">
         <v>625</v>
       </c>
@@ -5479,7 +5485,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="33"/>
       <c r="B38" s="2" t="s">
         <v>591</v>
@@ -5497,7 +5503,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="34"/>
       <c r="B39" s="2" t="s">
         <v>593</v>
@@ -5515,7 +5521,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="30" t="s">
         <v>547</v>
       </c>
@@ -5535,7 +5541,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="30"/>
       <c r="B42" s="2" t="s">
         <v>473</v>
@@ -5553,7 +5559,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="30" t="s">
         <v>627</v>
       </c>
@@ -5573,7 +5579,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="30"/>
       <c r="B45" s="2" t="s">
         <v>479</v>
@@ -5591,7 +5597,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="30"/>
       <c r="B46" s="2" t="s">
         <v>549</v>
@@ -5609,10 +5615,10 @@
         <v>551</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="25"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="30" t="s">
         <v>626</v>
       </c>
@@ -5632,7 +5638,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="30"/>
       <c r="B49" s="2" t="s">
         <v>483</v>
@@ -5650,7 +5656,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="30" t="s">
         <v>544</v>
       </c>
@@ -5670,7 +5676,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="30"/>
       <c r="B52" s="1" t="s">
         <v>491</v>
@@ -5688,7 +5694,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="30"/>
       <c r="B53" s="1" t="s">
         <v>495</v>
@@ -5706,7 +5712,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="30"/>
       <c r="B54" s="1" t="s">
         <v>499</v>
@@ -5724,7 +5730,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="30"/>
       <c r="B55" s="1" t="s">
         <v>552</v>
@@ -5742,7 +5748,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="30"/>
       <c r="B56" s="1" t="s">
         <v>504</v>
@@ -5760,7 +5766,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>631</v>
       </c>
@@ -5780,7 +5786,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="23" t="s">
         <v>634</v>
       </c>
@@ -5800,7 +5806,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="30" t="s">
         <v>629</v>
       </c>
@@ -5820,7 +5826,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="30"/>
       <c r="B63" s="2" t="s">
         <v>515</v>
@@ -5838,7 +5844,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="30"/>
       <c r="B64" s="2" t="s">
         <v>518</v>
@@ -5856,7 +5862,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="30"/>
       <c r="B65" s="2" t="s">
         <v>521</v>
@@ -5874,7 +5880,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="30"/>
       <c r="B66" s="2" t="s">
         <v>524</v>
@@ -5892,7 +5898,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="30"/>
       <c r="B67" s="2" t="s">
         <v>527</v>
@@ -5910,7 +5916,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="30"/>
       <c r="B68" s="2" t="s">
         <v>530</v>
@@ -5928,7 +5934,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="30"/>
       <c r="B69" s="2" t="s">
         <v>534</v>
@@ -5946,7 +5952,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="30"/>
       <c r="B70" s="2" t="s">
         <v>539</v>
@@ -5964,7 +5970,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="30" t="s">
         <v>633</v>
       </c>
@@ -5984,7 +5990,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="30"/>
       <c r="B73" s="2" t="s">
         <v>555</v>
@@ -6002,7 +6008,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="30"/>
       <c r="B74" s="2" t="s">
         <v>557</v>
@@ -6020,7 +6026,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>630</v>
       </c>
@@ -6040,7 +6046,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="30" t="s">
         <v>632</v>
       </c>
@@ -6060,7 +6066,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="30"/>
       <c r="B79" s="2" t="s">
         <v>608</v>
@@ -6080,6 +6086,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A28:A30"/>
     <mergeCell ref="A78:A79"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A44:A46"/>
@@ -6087,12 +6099,6 @@
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A72:A74"/>
     <mergeCell ref="A62:A70"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>